<commit_message>
Harmonize Datenlieferant and Datenowner
Museum Rietberg, Präsidialdepartement
</commit_message>
<xml_diff>
--- a/automation/mrz_himmelheber/Meta_Himmelheber_Objekte.xlsx
+++ b/automation/mrz_himmelheber/Meta_Himmelheber_Objekte.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Kura_KV\02_Kuratorium\03 Sammlung\07 Sammlungsdatenbank\Applikation\Externe_Sammlungszugaenge\Open Data\OGD\Objektarchiv Himmelheber\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszgua\Python\git\opendatazurich.github.io\automation\mrz_himmelheber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F3A8B7-565F-4249-92ED-9C3BCE95265B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D98E5F1-2103-4326-A015-6BF831B1BCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4260" yWindow="-20175" windowWidth="33000" windowHeight="18585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="1845" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="14" r:id="rId1"/>
@@ -962,9 +962,6 @@
 </t>
   </si>
   <si>
-    <t>Museum Rietberg Zürich, Präsidialdepartement</t>
-  </si>
-  <si>
     <t>Creditline</t>
   </si>
   <si>
@@ -1108,6 +1105,9 @@
   </si>
   <si>
     <t>Objekte, Maske, Archiv, Kunst, Gebrauchsgegenstände, Ethnologie, Reisen, Sammlung, Himmelheber, Afrika, Alaska</t>
+  </si>
+  <si>
+    <t>Museum Rietberg, Präsidialdepartement</t>
   </si>
 </sst>
 </file>
@@ -1847,23 +1847,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" style="11" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="66.83203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="53.58203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="66.875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="53.625" style="5" customWidth="1"/>
     <col min="5" max="5" width="8.75" style="5" customWidth="1"/>
-    <col min="6" max="6" width="88.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="50.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="88.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="50.375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="255.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
@@ -1897,14 +1897,14 @@
         <v>14</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>54</v>
       </c>
@@ -1915,14 +1915,14 @@
         <v>14</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
@@ -1933,14 +1933,14 @@
         <v>14</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
@@ -1967,14 +1967,14 @@
         <v>14</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>31</v>
       </c>
@@ -1985,14 +1985,14 @@
         <v>14</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>165</v>
+        <v>212</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -2003,14 +2003,14 @@
         <v>14</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>165</v>
+        <v>212</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>33</v>
       </c>
@@ -2021,14 +2021,14 @@
         <v>14</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>34</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>35</v>
       </c>
@@ -2055,14 +2055,14 @@
         <v>15</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -2073,14 +2073,14 @@
         <v>15</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>38</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>39</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>49</v>
       </c>
@@ -2127,14 +2127,14 @@
         <v>14</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>52</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="35" t="s">
         <v>130</v>
       </c>
@@ -2170,14 +2170,14 @@
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>37</v>
       </c>
@@ -2190,7 +2190,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="13" t="s">
         <v>11</v>
       </c>
@@ -2200,15 +2200,15 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="137.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="7"/>
@@ -2216,29 +2216,29 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" ht="43" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="43.5" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="7"/>
@@ -2246,46 +2246,46 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B24" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>171</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>172</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>164</v>
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="24"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D26" s="24"/>
       <c r="E26" s="7"/>
       <c r="F26" s="24"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="1"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="1"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2293,7 +2293,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>29</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="13" t="s">
         <v>26</v>
@@ -2327,25 +2327,25 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>30</v>
       </c>
@@ -2356,137 +2356,137 @@
         <v>11</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:6" s="4" customFormat="1" ht="50" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:6" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" s="4" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:6" s="4" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:6" s="4" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:6" s="4" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>30</v>
       </c>
@@ -2497,41 +2497,41 @@
         <v>40</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:6" s="4" customFormat="1" ht="50" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:6" s="4" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>30</v>
       </c>
@@ -2540,7 +2540,7 @@
       <c r="D45" s="22"/>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:6" s="4" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>30</v>
       </c>
@@ -2549,28 +2549,28 @@
       <c r="D46" s="22"/>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="11"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="11"/>
       <c r="B50" s="3" t="s">
         <v>161</v>
@@ -2579,14 +2579,14 @@
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="11"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>157</v>
       </c>
@@ -2600,7 +2600,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" ht="25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B53" s="13" t="s">
         <v>158</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
@@ -2634,131 +2634,131 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.375" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.25" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.58203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.58203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.08203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.58203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.375" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.375" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.875" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.625" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.375" style="25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.75" style="25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.58203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.625" style="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.875" style="25" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="34" t="s">
         <v>129</v>
       </c>
@@ -2780,14 +2780,14 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="5.58203125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="5.625" style="25" customWidth="1"/>
     <col min="3" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>71</v>
       </c>
@@ -2795,27 +2795,27 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>72</v>
       </c>
@@ -2823,12 +2823,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="34" t="s">
         <v>129</v>
       </c>
@@ -2850,14 +2850,14 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.375" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.25" style="25" customWidth="1"/>
     <col min="3" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>71</v>
       </c>
@@ -2865,118 +2865,118 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
     </row>
-    <row r="19" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="34" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
     </row>
-    <row r="23" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
     </row>
-    <row r="24" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
     </row>
-    <row r="25" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
     </row>
-    <row r="26" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
     </row>
-    <row r="27" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
     </row>
   </sheetData>
@@ -2996,15 +2996,15 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="58.58203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" style="25" customWidth="1"/>
+    <col min="3" max="3" width="58.625" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>71</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>88</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>89</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>90</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>91</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
         <v>92</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
         <v>93</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="28" t="s">
         <v>94</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
         <v>95</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
         <v>96</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
         <v>97</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
         <v>98</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
         <v>99</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>100</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
         <v>101</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
         <v>102</v>
       </c>
@@ -3195,12 +3195,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
         <v>129</v>
       </c>
@@ -3217,21 +3217,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008CBAF0EEED2F5B4AB4463B97C2AD2B71" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d2bc9691d179cb44d4ba77bdf8fcfb4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c4a6dd5ef775a5269b08f7de37f93f">
     <xsd:element name="properties">
@@ -3345,10 +3330,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3369,17 +3377,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>